<commit_message>
docs(work diary): update work diary of 18.09.2024
</commit_message>
<xml_diff>
--- a/documentation/Journal-de-Travail_Berchel-Joachim.xlsx
+++ b/documentation/Journal-de-Travail_Berchel-Joachim.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\px59nyu\Documents\GitHub\347-docker-swarm-wordpress\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A80CC1D-688C-4BC2-894C-DC3ABB06D79D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{685A9229-C659-4FA4-9632-FE685774C6E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
   <si>
     <t>Auteur:</t>
   </si>
@@ -146,6 +146,24 @@
   </si>
   <si>
     <t>Docker Swarm Wordpress - 347</t>
+  </si>
+  <si>
+    <t>Repréparer le travail à effectuer et informer mon camarade de ce qu'il faut faire</t>
+  </si>
+  <si>
+    <t>Se connecter par SSH</t>
+  </si>
+  <si>
+    <t>Créer les VM</t>
+  </si>
+  <si>
+    <t>Connexion par SSH pour le NFS, au final je n'ai rien fais d'autre</t>
+  </si>
+  <si>
+    <t>J'essaie de me connecter à une des machines distantes. Sans réussite. Permission denied (publickey).</t>
+  </si>
+  <si>
+    <t>J'essaie de connecter nginx à worpress en local. Sans succès</t>
   </si>
 </sst>
 </file>
@@ -1085,10 +1103,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>60</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30</c:v>
+                  <c:v>170</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1937,10 +1955,10 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.66666666666666663</c:v>
+                  <c:v>0.30612244897959184</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.33333333333333331</c:v>
+                  <c:v>0.69387755102040816</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -4132,7 +4150,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4187,7 +4205,7 @@
       <c r="B3" s="82"/>
       <c r="C3" s="78" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>1 heures 30 minutes</v>
+        <v>4 heures 5 minutes</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="3"/>
@@ -4206,11 +4224,11 @@
       </c>
       <c r="D4" s="19">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>90</v>
+        <v>245</v>
       </c>
       <c r="E4" s="29">
         <f>SUM(C4:D4)</f>
-        <v>90</v>
+        <v>245</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4352,15 +4370,23 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="74" t="str">
+      <c r="A11" s="74">
         <f>IF(ISBLANK(B11),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B11))</f>
-        <v/>
-      </c>
-      <c r="B11" s="40"/>
+        <v>38</v>
+      </c>
+      <c r="B11" s="40">
+        <v>45553</v>
+      </c>
       <c r="C11" s="41"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="28"/>
+      <c r="D11" s="42">
+        <v>15</v>
+      </c>
+      <c r="E11" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>35</v>
+      </c>
       <c r="G11" s="46"/>
       <c r="M11" t="s">
         <v>4</v>
@@ -4373,15 +4399,23 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="73" t="str">
+      <c r="A12" s="73">
         <f>IF(ISBLANK(B12),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B12))</f>
-        <v/>
-      </c>
-      <c r="B12" s="36"/>
+        <v>38</v>
+      </c>
+      <c r="B12" s="36">
+        <v>45553</v>
+      </c>
       <c r="C12" s="37"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="28"/>
+      <c r="D12" s="38">
+        <v>40</v>
+      </c>
+      <c r="E12" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>36</v>
+      </c>
       <c r="G12" s="45"/>
       <c r="N12">
         <v>5</v>
@@ -4391,15 +4425,23 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="74" t="str">
+      <c r="A13" s="74">
         <f>IF(ISBLANK(B13),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B13))</f>
-        <v/>
-      </c>
-      <c r="B13" s="40"/>
+        <v>38</v>
+      </c>
+      <c r="B13" s="40">
+        <v>45553</v>
+      </c>
       <c r="C13" s="41"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="28"/>
+      <c r="D13" s="42">
+        <v>10</v>
+      </c>
+      <c r="E13" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="28" t="s">
+        <v>37</v>
+      </c>
       <c r="G13" s="46"/>
       <c r="N13">
         <v>6</v>
@@ -4409,15 +4451,23 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="73" t="str">
+      <c r="A14" s="73">
         <f>IF(ISBLANK(B14),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B14))</f>
-        <v/>
-      </c>
-      <c r="B14" s="36"/>
+        <v>38</v>
+      </c>
+      <c r="B14" s="36">
+        <v>45553</v>
+      </c>
       <c r="C14" s="37"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="28"/>
+      <c r="D14" s="38">
+        <v>30</v>
+      </c>
+      <c r="E14" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="28" t="s">
+        <v>38</v>
+      </c>
       <c r="G14" s="45"/>
       <c r="N14">
         <v>7</v>
@@ -4426,16 +4476,24 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="74" t="str">
+    <row r="15" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="74">
         <f>IF(ISBLANK(B15),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B15))</f>
-        <v/>
-      </c>
-      <c r="B15" s="40"/>
+        <v>38</v>
+      </c>
+      <c r="B15" s="40">
+        <v>45553</v>
+      </c>
       <c r="C15" s="41"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="43"/>
-      <c r="F15" s="28"/>
+      <c r="D15" s="42">
+        <v>15</v>
+      </c>
+      <c r="E15" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="28" t="s">
+        <v>39</v>
+      </c>
       <c r="G15" s="46"/>
       <c r="N15">
         <v>8</v>
@@ -4445,15 +4503,23 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="73" t="str">
+      <c r="A16" s="73">
         <f>IF(ISBLANK(B16),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B16))</f>
-        <v/>
-      </c>
-      <c r="B16" s="36"/>
+        <v>38</v>
+      </c>
+      <c r="B16" s="36">
+        <v>45553</v>
+      </c>
       <c r="C16" s="37"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="28"/>
+      <c r="D16" s="38">
+        <v>45</v>
+      </c>
+      <c r="E16" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="28" t="s">
+        <v>40</v>
+      </c>
       <c r="G16" s="45"/>
       <c r="O16">
         <v>40</v>
@@ -10719,7 +10785,7 @@
   <dimension ref="A2:N12"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -10800,11 +10866,11 @@
       </c>
       <c r="B6">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E6,'Journal de travail'!$D$7:$D$532)</f>
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="C6">
         <f t="shared" ref="C6:C9" si="0">SUM(A6:B6)</f>
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="E6" s="21" t="str">
         <f>'Journal de travail'!M8</f>
@@ -10812,11 +10878,11 @@
       </c>
       <c r="F6" s="50" t="str">
         <f>QUOTIENT(SUM(A6:B6),60)&amp;" h "&amp;TEXT(MOD(SUM(A6:B6),60), "00")&amp;" min"</f>
-        <v>1 h 00 min</v>
+        <v>1 h 15 min</v>
       </c>
       <c r="G6" s="47">
         <f>SUM(A6:B6)/$C$10</f>
-        <v>0.66666666666666663</v>
+        <v>0.30612244897959184</v>
       </c>
       <c r="L6" s="62" t="str">
         <f>'Journal de travail'!M8</f>
@@ -10837,11 +10903,11 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>30</v>
+        <v>170</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>170</v>
       </c>
       <c r="E7" s="30" t="str">
         <f>'Journal de travail'!M9</f>
@@ -10849,11 +10915,11 @@
       </c>
       <c r="F7" s="55" t="str">
         <f t="shared" ref="F7:F10" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>0 h 30 min</v>
+        <v>2 h 50 min</v>
       </c>
       <c r="G7" s="56">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$10</f>
-        <v>0.33333333333333331</v>
+        <v>0.69387755102040816</v>
       </c>
       <c r="L7" s="64" t="str">
         <f>'Journal de travail'!M9</f>
@@ -10948,22 +11014,22 @@
       </c>
       <c r="B10">
         <f>SUM(B6:B9)</f>
-        <v>90</v>
+        <v>245</v>
       </c>
       <c r="C10">
         <f>SUM(A10:B10)</f>
-        <v>90</v>
+        <v>245</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>1 h 30 min</v>
+        <v>4 h 05 min</v>
       </c>
       <c r="G10" s="57">
         <f>C10/C11</f>
-        <v>1.7045454545454544E-2</v>
+        <v>4.6401515151515152E-2</v>
       </c>
       <c r="L10" s="67" t="s">
         <v>18</v>
@@ -10994,7 +11060,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67F31118-7D2C-C547-B9C9-EA2B04E048B8}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="R36" sqref="R36"/>
     </sheetView>
   </sheetViews>
@@ -11007,26 +11073,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -11249,26 +11295,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11285,4 +11332,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
docs(work diary): update the work diary of 05.10.2024
</commit_message>
<xml_diff>
--- a/documentation/Journal-de-Travail_Berchel-Joachim.xlsx
+++ b/documentation/Journal-de-Travail_Berchel-Joachim.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\px59nyu\Documents\GitHub\347-docker-swarm-wordpress\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67BDAE27-5F72-44F3-A2C6-728924CEFF0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B469C411-FCC0-455E-9DFA-ACAA2105E564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="53">
   <si>
     <t>Auteur:</t>
   </si>
@@ -191,6 +191,15 @@
   </si>
   <si>
     <t>J'essaie de régler l'erreur 403, Thomas m'aide</t>
+  </si>
+  <si>
+    <t>Je mets en place mon environnement de travail. Forticlient ne fonctionne pas</t>
+  </si>
+  <si>
+    <t>Fais lors d'une convocation un Samedi</t>
+  </si>
+  <si>
+    <t>J'essaie de lancer ma stack, erreur "File not found"</t>
   </si>
 </sst>
 </file>
@@ -1133,7 +1142,7 @@
                   <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>555</c:v>
+                  <c:v>645</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1982,10 +1991,10 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.11904761904761904</c:v>
+                  <c:v>0.10416666666666667</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.88095238095238093</c:v>
+                  <c:v>0.89583333333333337</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -4177,7 +4186,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
+      <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4232,7 +4241,7 @@
       <c r="B3" s="82"/>
       <c r="C3" s="78" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>10 heures 50 minutes</v>
+        <v>12 heures 20 minutes</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="3"/>
@@ -4247,15 +4256,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="19">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>180</v>
+        <v>240</v>
       </c>
       <c r="D4" s="19">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>470</v>
+        <v>500</v>
       </c>
       <c r="E4" s="29">
         <f>SUM(C4:D4)</f>
-        <v>650</v>
+        <v>740</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4726,27 +4735,45 @@
       <c r="G24" s="45"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="74" t="str">
+      <c r="A25" s="74">
         <f>IF(ISBLANK(B25),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B25))</f>
-        <v/>
-      </c>
-      <c r="B25" s="40"/>
+        <v>40</v>
+      </c>
+      <c r="B25" s="40">
+        <v>45570</v>
+      </c>
       <c r="C25" s="41"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="43"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="46"/>
+      <c r="D25" s="42">
+        <v>30</v>
+      </c>
+      <c r="E25" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F25" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="G25" s="46" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="73" t="str">
+      <c r="A26" s="73">
         <f>IF(ISBLANK(B26),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B26))</f>
-        <v/>
-      </c>
-      <c r="B26" s="36"/>
-      <c r="C26" s="37"/>
+        <v>40</v>
+      </c>
+      <c r="B26" s="36">
+        <v>45570</v>
+      </c>
+      <c r="C26" s="37">
+        <v>1</v>
+      </c>
       <c r="D26" s="38"/>
-      <c r="E26" s="39"/>
-      <c r="F26" s="28"/>
+      <c r="E26" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26" s="28" t="s">
+        <v>52</v>
+      </c>
       <c r="G26" s="45"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
@@ -10977,7 +11004,7 @@
       </c>
       <c r="G6" s="47">
         <f>SUM(A6:B6)/$C$10</f>
-        <v>0.11904761904761904</v>
+        <v>0.10416666666666667</v>
       </c>
       <c r="L6" s="62" t="str">
         <f>'Journal de travail'!M8</f>
@@ -10994,15 +11021,15 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>180</v>
+        <v>240</v>
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>375</v>
+        <v>405</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>555</v>
+        <v>645</v>
       </c>
       <c r="E7" s="30" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11010,11 +11037,11 @@
       </c>
       <c r="F7" s="55" t="str">
         <f t="shared" ref="F7:F10" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>9 h 15 min</v>
+        <v>10 h 45 min</v>
       </c>
       <c r="G7" s="56">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$10</f>
-        <v>0.88095238095238093</v>
+        <v>0.89583333333333337</v>
       </c>
       <c r="L7" s="64" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11105,26 +11132,26 @@
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <f>SUM(A6:A9)</f>
-        <v>180</v>
+        <v>240</v>
       </c>
       <c r="B10">
         <f>SUM(B6:B9)</f>
-        <v>450</v>
+        <v>480</v>
       </c>
       <c r="C10">
         <f>SUM(A10:B10)</f>
-        <v>630</v>
+        <v>720</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>10 h 30 min</v>
+        <v>12 h 00 min</v>
       </c>
       <c r="G10" s="57">
         <f>C10/C11</f>
-        <v>0.11931818181818182</v>
+        <v>0.13636363636363635</v>
       </c>
       <c r="L10" s="67" t="s">
         <v>18</v>
@@ -11168,6 +11195,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -11390,27 +11437,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11427,23 +11473,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
docs(work diary): update work diary of 07.10.2024
</commit_message>
<xml_diff>
--- a/documentation/Journal-de-Travail_Berchel-Joachim.xlsx
+++ b/documentation/Journal-de-Travail_Berchel-Joachim.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\px59nyu\Documents\GitHub\347-docker-swarm-wordpress\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B469C411-FCC0-455E-9DFA-ACAA2105E564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8950AAB-983E-4968-B8EF-11B65CF2591F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="55">
   <si>
     <t>Auteur:</t>
   </si>
@@ -200,6 +200,12 @@
   </si>
   <si>
     <t>J'essaie de lancer ma stack, erreur "File not found"</t>
+  </si>
+  <si>
+    <t>On a réussi à se connecter à nginx</t>
+  </si>
+  <si>
+    <t>Erreur database</t>
   </si>
 </sst>
 </file>
@@ -1142,7 +1148,7 @@
                   <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>645</c:v>
+                  <c:v>815</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1991,10 +1997,10 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.10416666666666667</c:v>
+                  <c:v>8.4269662921348312E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.89583333333333337</c:v>
+                  <c:v>0.9157303370786517</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -4186,7 +4192,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
+      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4241,7 +4247,7 @@
       <c r="B3" s="82"/>
       <c r="C3" s="78" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>12 heures 20 minutes</v>
+        <v>15 heures 10 minutes</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="3"/>
@@ -4256,15 +4262,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="19">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>240</v>
+        <v>360</v>
       </c>
       <c r="D4" s="19">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>500</v>
+        <v>550</v>
       </c>
       <c r="E4" s="29">
         <f>SUM(C4:D4)</f>
-        <v>740</v>
+        <v>910</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4777,27 +4783,45 @@
       <c r="G26" s="45"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="74" t="str">
+      <c r="A27" s="74">
         <f>IF(ISBLANK(B27),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B27))</f>
-        <v/>
-      </c>
-      <c r="B27" s="40"/>
-      <c r="C27" s="41"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="43"/>
-      <c r="F27" s="28"/>
+        <v>41</v>
+      </c>
+      <c r="B27" s="40">
+        <v>45572</v>
+      </c>
+      <c r="C27" s="41">
+        <v>2</v>
+      </c>
+      <c r="D27" s="42">
+        <v>30</v>
+      </c>
+      <c r="E27" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" s="28" t="s">
+        <v>53</v>
+      </c>
       <c r="G27" s="46"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="73" t="str">
+      <c r="A28" s="73">
         <f>IF(ISBLANK(B28),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B28))</f>
-        <v/>
-      </c>
-      <c r="B28" s="36"/>
+        <v>41</v>
+      </c>
+      <c r="B28" s="36">
+        <v>45572</v>
+      </c>
       <c r="C28" s="37"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="39"/>
-      <c r="F28" s="27"/>
+      <c r="D28" s="38">
+        <v>20</v>
+      </c>
+      <c r="E28" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F28" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="G28" s="45"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
@@ -11004,7 +11028,7 @@
       </c>
       <c r="G6" s="47">
         <f>SUM(A6:B6)/$C$10</f>
-        <v>0.10416666666666667</v>
+        <v>8.4269662921348312E-2</v>
       </c>
       <c r="L6" s="62" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11021,15 +11045,15 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>240</v>
+        <v>360</v>
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>405</v>
+        <v>455</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>645</v>
+        <v>815</v>
       </c>
       <c r="E7" s="30" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11037,11 +11061,11 @@
       </c>
       <c r="F7" s="55" t="str">
         <f t="shared" ref="F7:F10" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>10 h 45 min</v>
+        <v>13 h 35 min</v>
       </c>
       <c r="G7" s="56">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$10</f>
-        <v>0.89583333333333337</v>
+        <v>0.9157303370786517</v>
       </c>
       <c r="L7" s="64" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11132,26 +11156,26 @@
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <f>SUM(A6:A9)</f>
-        <v>240</v>
+        <v>360</v>
       </c>
       <c r="B10">
         <f>SUM(B6:B9)</f>
-        <v>480</v>
+        <v>530</v>
       </c>
       <c r="C10">
         <f>SUM(A10:B10)</f>
-        <v>720</v>
+        <v>890</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>12 h 00 min</v>
+        <v>14 h 50 min</v>
       </c>
       <c r="G10" s="57">
         <f>C10/C11</f>
-        <v>0.13636363636363635</v>
+        <v>0.16856060606060605</v>
       </c>
       <c r="L10" s="67" t="s">
         <v>18</v>
@@ -11195,26 +11219,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -11437,26 +11441,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11473,4 +11478,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
docs(work diary): update work diary of 09.10.2024
</commit_message>
<xml_diff>
--- a/documentation/Journal-de-Travail_Berchel-Joachim.xlsx
+++ b/documentation/Journal-de-Travail_Berchel-Joachim.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\px59nyu\Documents\GitHub\347-docker-swarm-wordpress\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8950AAB-983E-4968-B8EF-11B65CF2591F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE41B63-DD2A-46A2-BD60-0BA27218B967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="57">
   <si>
     <t>Auteur:</t>
   </si>
@@ -206,6 +206,12 @@
   </si>
   <si>
     <t>Erreur database</t>
+  </si>
+  <si>
+    <t>Je commente le code, en essayant quelque chose avec wordpress j'ai cassé les services, wordpress ne fonctionne plus et swarmpit non plus. Lucas a réglé le problème</t>
+  </si>
+  <si>
+    <t>Je vérifie que le code sur les machines distantes soit les mêmes que le code sur Github</t>
   </si>
 </sst>
 </file>
@@ -1148,7 +1154,7 @@
                   <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>815</c:v>
+                  <c:v>925</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1997,10 +2003,10 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>8.4269662921348312E-2</c:v>
+                  <c:v>7.4999999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.9157303370786517</c:v>
+                  <c:v>0.92500000000000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -4191,8 +4197,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
+      <pane ySplit="6" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4247,7 +4253,7 @@
       <c r="B3" s="82"/>
       <c r="C3" s="78" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>15 heures 10 minutes</v>
+        <v>17 heures 0 minutes</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="3"/>
@@ -4262,15 +4268,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="19">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>360</v>
+        <v>420</v>
       </c>
       <c r="D4" s="19">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>550</v>
+        <v>600</v>
       </c>
       <c r="E4" s="29">
         <f>SUM(C4:D4)</f>
-        <v>910</v>
+        <v>1020</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4825,27 +4831,45 @@
       <c r="G28" s="45"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="74" t="str">
+      <c r="A29" s="74">
         <f>IF(ISBLANK(B29),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B29))</f>
-        <v/>
-      </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="41"/>
-      <c r="D29" s="42"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="27"/>
+        <v>41</v>
+      </c>
+      <c r="B29" s="40">
+        <v>45574</v>
+      </c>
+      <c r="C29" s="41">
+        <v>1</v>
+      </c>
+      <c r="D29" s="42">
+        <v>20</v>
+      </c>
+      <c r="E29" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F29" s="27" t="s">
+        <v>55</v>
+      </c>
       <c r="G29" s="46"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="73" t="str">
+      <c r="A30" s="73">
         <f>IF(ISBLANK(B30),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B30))</f>
-        <v/>
-      </c>
-      <c r="B30" s="36"/>
+        <v>41</v>
+      </c>
+      <c r="B30" s="36">
+        <v>45574</v>
+      </c>
       <c r="C30" s="37"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="39"/>
-      <c r="F30" s="28"/>
+      <c r="D30" s="38">
+        <v>30</v>
+      </c>
+      <c r="E30" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F30" s="28" t="s">
+        <v>56</v>
+      </c>
       <c r="G30" s="45"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
@@ -11028,7 +11052,7 @@
       </c>
       <c r="G6" s="47">
         <f>SUM(A6:B6)/$C$10</f>
-        <v>8.4269662921348312E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="L6" s="62" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11045,15 +11069,15 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>360</v>
+        <v>420</v>
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>455</v>
+        <v>505</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>815</v>
+        <v>925</v>
       </c>
       <c r="E7" s="30" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11061,11 +11085,11 @@
       </c>
       <c r="F7" s="55" t="str">
         <f t="shared" ref="F7:F10" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>13 h 35 min</v>
+        <v>15 h 25 min</v>
       </c>
       <c r="G7" s="56">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$10</f>
-        <v>0.9157303370786517</v>
+        <v>0.92500000000000004</v>
       </c>
       <c r="L7" s="64" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11156,26 +11180,26 @@
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <f>SUM(A6:A9)</f>
-        <v>360</v>
+        <v>420</v>
       </c>
       <c r="B10">
         <f>SUM(B6:B9)</f>
-        <v>530</v>
+        <v>580</v>
       </c>
       <c r="C10">
         <f>SUM(A10:B10)</f>
-        <v>890</v>
+        <v>1000</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>14 h 50 min</v>
+        <v>16 h 40 min</v>
       </c>
       <c r="G10" s="57">
         <f>C10/C11</f>
-        <v>0.16856060606060605</v>
+        <v>0.18939393939393939</v>
       </c>
       <c r="L10" s="67" t="s">
         <v>18</v>
@@ -11219,6 +11243,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -11441,27 +11485,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11478,23 +11521,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
docs(work diary): update the work diary of the 30.10.2024
</commit_message>
<xml_diff>
--- a/documentation/Journal-de-Travail_Berchel-Joachim.xlsx
+++ b/documentation/Journal-de-Travail_Berchel-Joachim.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\px59nyu\Documents\GitHub\347-docker-swarm-wordpress\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE41B63-DD2A-46A2-BD60-0BA27218B967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA00A4E-70B6-4DC2-ADA6-3BD5F9431670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="59">
   <si>
     <t>Auteur:</t>
   </si>
@@ -212,6 +212,12 @@
   </si>
   <si>
     <t>Je vérifie que le code sur les machines distantes soit les mêmes que le code sur Github</t>
+  </si>
+  <si>
+    <t>Vérifier le README, les fichiers/dossier inutiles</t>
+  </si>
+  <si>
+    <t>Vérifier que la version local du docker fonctionne.</t>
   </si>
 </sst>
 </file>
@@ -1151,10 +1157,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>75</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>925</c:v>
+                  <c:v>1015</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2003,10 +2009,10 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>7.4999999999999997E-2</c:v>
+                  <c:v>9.7777777777777783E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.92500000000000004</c:v>
+                  <c:v>0.90222222222222226</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -4197,8 +4203,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F31" sqref="F31"/>
+      <pane ySplit="6" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4253,7 +4259,7 @@
       <c r="B3" s="82"/>
       <c r="C3" s="78" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>17 heures 0 minutes</v>
+        <v>19 heures 5 minutes</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="3"/>
@@ -4268,15 +4274,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="19">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>420</v>
+        <v>480</v>
       </c>
       <c r="D4" s="19">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>600</v>
+        <v>665</v>
       </c>
       <c r="E4" s="29">
         <f>SUM(C4:D4)</f>
-        <v>1020</v>
+        <v>1145</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4873,15 +4879,23 @@
       <c r="G30" s="45"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="74" t="str">
+      <c r="A31" s="74">
         <f>IF(ISBLANK(B31),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B31))</f>
-        <v/>
-      </c>
-      <c r="B31" s="40"/>
+        <v>44</v>
+      </c>
+      <c r="B31" s="40">
+        <v>45595</v>
+      </c>
       <c r="C31" s="41"/>
-      <c r="D31" s="42"/>
-      <c r="E31" s="43"/>
-      <c r="F31" s="27"/>
+      <c r="D31" s="42">
+        <v>35</v>
+      </c>
+      <c r="E31" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="F31" s="27" t="s">
+        <v>57</v>
+      </c>
       <c r="G31" s="46"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
@@ -4890,10 +4904,18 @@
         <v/>
       </c>
       <c r="B32" s="36"/>
-      <c r="C32" s="37"/>
-      <c r="D32" s="38"/>
-      <c r="E32" s="39"/>
-      <c r="F32" s="28"/>
+      <c r="C32" s="37">
+        <v>1</v>
+      </c>
+      <c r="D32" s="38">
+        <v>30</v>
+      </c>
+      <c r="E32" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F32" s="28" t="s">
+        <v>58</v>
+      </c>
       <c r="G32" s="45"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -11036,11 +11058,11 @@
       </c>
       <c r="B6">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E6,'Journal de travail'!$D$7:$D$532)</f>
-        <v>75</v>
+        <v>110</v>
       </c>
       <c r="C6">
         <f t="shared" ref="C6:C9" si="0">SUM(A6:B6)</f>
-        <v>75</v>
+        <v>110</v>
       </c>
       <c r="E6" s="21" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11048,11 +11070,11 @@
       </c>
       <c r="F6" s="50" t="str">
         <f>QUOTIENT(SUM(A6:B6),60)&amp;" h "&amp;TEXT(MOD(SUM(A6:B6),60), "00")&amp;" min"</f>
-        <v>1 h 15 min</v>
+        <v>1 h 50 min</v>
       </c>
       <c r="G6" s="47">
         <f>SUM(A6:B6)/$C$10</f>
-        <v>7.4999999999999997E-2</v>
+        <v>9.7777777777777783E-2</v>
       </c>
       <c r="L6" s="62" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11069,15 +11091,15 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>420</v>
+        <v>480</v>
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>505</v>
+        <v>535</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>925</v>
+        <v>1015</v>
       </c>
       <c r="E7" s="30" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11085,11 +11107,11 @@
       </c>
       <c r="F7" s="55" t="str">
         <f t="shared" ref="F7:F10" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>15 h 25 min</v>
+        <v>16 h 55 min</v>
       </c>
       <c r="G7" s="56">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$10</f>
-        <v>0.92500000000000004</v>
+        <v>0.90222222222222226</v>
       </c>
       <c r="L7" s="64" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11180,26 +11202,26 @@
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <f>SUM(A6:A9)</f>
-        <v>420</v>
+        <v>480</v>
       </c>
       <c r="B10">
         <f>SUM(B6:B9)</f>
-        <v>580</v>
+        <v>645</v>
       </c>
       <c r="C10">
         <f>SUM(A10:B10)</f>
-        <v>1000</v>
+        <v>1125</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>16 h 40 min</v>
+        <v>18 h 45 min</v>
       </c>
       <c r="G10" s="57">
         <f>C10/C11</f>
-        <v>0.18939393939393939</v>
+        <v>0.21306818181818182</v>
       </c>
       <c r="L10" s="67" t="s">
         <v>18</v>
@@ -11243,26 +11265,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -11485,26 +11487,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11521,4 +11524,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>